<commit_message>
made changes according to WA Beta
</commit_message>
<xml_diff>
--- a/architect_contacts.xlsx
+++ b/architect_contacts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\resinfinity_architect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4573EF56-7464-4830-AF98-958F25FDEE48}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9CE9D2-9FFE-47BD-9F4C-294137F42527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5328" yWindow="48" windowWidth="11736" windowHeight="12312" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -360,7 +360,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -404,18 +404,18 @@
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="6">
-        <v>7043158100</v>
+        <v>1111111111</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="6">
-        <v>1111111111</v>
+        <v>7043158100</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>